<commit_message>
Test Broken Images v1.0.0
</commit_message>
<xml_diff>
--- a/Plan de pruebas/Plan de pruebas - The internet.xlsx
+++ b/Plan de pruebas/Plan de pruebas - The internet.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4575"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan de pruebas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Titulo del caso de prueba</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Comentarios</t>
-  </si>
-  <si>
-    <t>A/B Testing</t>
   </si>
   <si>
     <t>1. Ingresar en la url "https://the-internet.herokuapp.com/"
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>No se presento ningun issue relacionado a la prueba</t>
-  </si>
-  <si>
-    <t>Add/Remove Elements</t>
   </si>
   <si>
     <t>1. Ingresar en la url "https://the-internet.herokuapp.com/"
@@ -81,9 +75,6 @@
     <t>CP-002</t>
   </si>
   <si>
-    <t>Basic Auth</t>
-  </si>
-  <si>
     <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
 2. Usar credenciales: User "admin", password "admin"
 3. Validar el correcto inicio de sesion</t>
@@ -93,6 +84,35 @@
   </si>
   <si>
     <t>CP-003</t>
+  </si>
+  <si>
+    <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
+2. Dar click a boton "Broken Image"
+3. Validar si existen imágenes que no cargan correctamente</t>
+  </si>
+  <si>
+    <t>CP-004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todas las imágenes de la pagina cargan correctamente  </t>
+  </si>
+  <si>
+    <t>Fallida</t>
+  </si>
+  <si>
+    <t>Issue: 2 de las imágenes no cargan correctamente</t>
+  </si>
+  <si>
+    <t>CP-001 A/B Testing</t>
+  </si>
+  <si>
+    <t>CP-002 Add/Remove Elements</t>
+  </si>
+  <si>
+    <t>CP-003 Basic Auth</t>
+  </si>
+  <si>
+    <t>CP-004 Broken Image</t>
   </si>
 </sst>
 </file>
@@ -318,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,12 +387,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -391,27 +414,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -694,7 +696,7 @@
   <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +706,7 @@
     <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -722,7 +724,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
@@ -730,71 +732,83 @@
     </row>
     <row r="3" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="F3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="101.25" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="E4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="F5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
@@ -1054,13 +1068,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F38">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Exitosa">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Exitosa">
       <formula>NOT(ISERROR(SEARCH("Exitosa",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Fallida">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fallida">
       <formula>NOT(ISERROR(SEARCH("Fallida",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Exitosa con observaciones">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Exitosa con observaciones">
       <formula>NOT(ISERROR(SEARCH("Exitosa con observaciones",F3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Plan de pruebas v1.0.1
</commit_message>
<xml_diff>
--- a/Plan de pruebas/Plan de pruebas - The internet.xlsx
+++ b/Plan de pruebas/Plan de pruebas - The internet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Titulo del caso de prueba</t>
   </si>
@@ -113,6 +113,38 @@
   </si>
   <si>
     <t>CP-004 Broken Image</t>
+  </si>
+  <si>
+    <t>CP-005 Checkboxes</t>
+  </si>
+  <si>
+    <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
+2. Dar click a boton "Checkboxes"
+3. Validar los 2 checkbox</t>
+  </si>
+  <si>
+    <t>Se puede marcar y desmarcar los 2 checkbox</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>CP-006 Contxt menu</t>
+  </si>
+  <si>
+    <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
+2. Dar click a boton "Context menu"
+3. Dar click derecho a la caja
+4. Validar el despliegue del menu de contexto</t>
+  </si>
+  <si>
+    <t>Al dar click derecho a la caja se despliega un menu contextual</t>
+  </si>
+  <si>
+    <t>CP-005</t>
+  </si>
+  <si>
+    <t>CP-006</t>
   </si>
 </sst>
 </file>
@@ -395,7 +427,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -414,6 +446,34 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -696,7 +756,7 @@
   <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,20 +870,40 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
+    <row r="7" spans="2:7" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
+    <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1068,14 +1148,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F38">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Exitosa">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Exitosa">
       <formula>NOT(ISERROR(SEARCH("Exitosa",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fallida">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Fallida">
       <formula>NOT(ISERROR(SEARCH("Fallida",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Exitosa con observaciones">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Exitosa con observaciones">
       <formula>NOT(ISERROR(SEARCH("Exitosa con observaciones",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="En proceso">
+      <formula>NOT(ISERROR(SEARCH("En proceso",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Plan de pruebas v1.0.2
</commit_message>
<xml_diff>
--- a/Plan de pruebas/Plan de pruebas - The internet.xlsx
+++ b/Plan de pruebas/Plan de pruebas - The internet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Titulo del caso de prueba</t>
   </si>
@@ -86,11 +86,6 @@
     <t>CP-003</t>
   </si>
   <si>
-    <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
-2. Dar click a boton "Broken Image"
-3. Validar si existen imágenes que no cargan correctamente</t>
-  </si>
-  <si>
     <t>CP-004</t>
   </si>
   <si>
@@ -98,9 +93,6 @@
   </si>
   <si>
     <t>Fallida</t>
-  </si>
-  <si>
-    <t>Issue: 2 de las imágenes no cargan correctamente</t>
   </si>
   <si>
     <t>CP-001 A/B Testing</t>
@@ -145,6 +137,50 @@
   </si>
   <si>
     <t>CP-006</t>
+  </si>
+  <si>
+    <t>Issues: 2 de las imágenes no cargan correctamente</t>
+  </si>
+  <si>
+    <t>CP-007 Drag and drop</t>
+  </si>
+  <si>
+    <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
+2. Dar click en boton "Drag and Drop"
+3. Validar que existe recuadro "A" y "B"
+3. Mover recuadro "A" al lugar de recuadro "B"
+4. Mover recuadro "A" a su posicion original
+5. Mover recuadro "B" a la posicion del recuadro "A"
+6. Mover recuadro "B" a su posicion original
+7. Validar que los movimientos se realizaron correctamente</t>
+  </si>
+  <si>
+    <t>1. Al mover el recuadro "A" a la posicion del recuadro "B" estos deben cambiar de posiciones y al mover nuevamente el recuadro "A" a su posicion anterior, ambos recuadros quedan en su posicion original
+2. Al mover el recuadro "B" a la posicion del recuadro "A" estos deben cambiar de posiciones y al mover nuevamente el recuadro "B" a su posicion anterior, ambos quedan en su posicion original</t>
+  </si>
+  <si>
+    <t>CP-007</t>
+  </si>
+  <si>
+    <t>CP-008 Dropdown list</t>
+  </si>
+  <si>
+    <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
+2. Dar click a boton "Broken Image"
+3. Validar que las imágenes carguen correctamente</t>
+  </si>
+  <si>
+    <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
+2. Dar click a boton "Drop List"
+3. Desplegar menu y seleccionar "Option 1"
+4. Desplegar menu y seleccionar "Option 2"
+5. Validar las opciones seleccionadas</t>
+  </si>
+  <si>
+    <t>El menu se debe desplegar y se deben poder seleccionar todas sus opciones</t>
+  </si>
+  <si>
+    <t>CP-008</t>
   </si>
 </sst>
 </file>
@@ -427,7 +463,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -446,34 +489,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -755,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +807,7 @@
     </row>
     <row r="3" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
@@ -812,7 +827,7 @@
     </row>
     <row r="4" spans="2:7" ht="101.25" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>11</v>
@@ -832,7 +847,7 @@
     </row>
     <row r="5" spans="2:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>14</v>
@@ -852,74 +867,98 @@
     </row>
     <row r="6" spans="2:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="F6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>20</v>
-      </c>
       <c r="G6" s="17" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="67.5" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="15"/>
+        <v>9</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
+    <row r="10" spans="2:7" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="G10" s="15"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1148,16 +1187,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F38">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Exitosa">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Exitosa">
       <formula>NOT(ISERROR(SEARCH("Exitosa",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Fallida">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Fallida">
       <formula>NOT(ISERROR(SEARCH("Fallida",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Exitosa con observaciones">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Exitosa con observaciones">
       <formula>NOT(ISERROR(SEARCH("Exitosa con observaciones",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="En proceso">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="En proceso">
       <formula>NOT(ISERROR(SEARCH("En proceso",F3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Plan de pruebas v1.0.3
</commit_message>
<xml_diff>
--- a/Plan de pruebas/Plan de pruebas - The internet.xlsx
+++ b/Plan de pruebas/Plan de pruebas - The internet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Titulo del caso de prueba</t>
   </si>
@@ -182,12 +182,40 @@
   <si>
     <t>CP-008</t>
   </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>CP-009 File downloader</t>
+  </si>
+  <si>
+    <t>1. Ingresar en la url "https://the-internet.herokuapp.com/basic_auth"
+2. Dar click a boton "File downloader"
+3. Dar click a cada boton en la pagina
+4. Descargar cada archivo
+5. Validar que se descargo correctamente</t>
+  </si>
+  <si>
+    <t>Se deben poder descargar cada archivo mostrado en la pagina</t>
+  </si>
+  <si>
+    <t>CP-009</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +245,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -238,7 +273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -402,11 +437,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -432,9 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -450,20 +495,84 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -494,6 +603,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFF00"/>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -768,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G38"/>
+  <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,8 +901,8 @@
     <col min="7" max="7" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -801,11 +918,14 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
@@ -818,386 +938,461 @@
       <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="H3" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="H4" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="H5" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="H6" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="H7" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="191.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="H8" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="2:7" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="G9" s="14"/>
+      <c r="H9" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="15"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="15"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="15"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="15"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="15"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="15"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="15"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="16"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="16"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="16"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="16"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F38">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Exitosa">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Exitosa">
       <formula>NOT(ISERROR(SEARCH("Exitosa",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Fallida">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Fallida">
       <formula>NOT(ISERROR(SEARCH("Fallida",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Exitosa con observaciones">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Exitosa con observaciones">
       <formula>NOT(ISERROR(SEARCH("Exitosa con observaciones",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="En proceso">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="En proceso">
       <formula>NOT(ISERROR(SEARCH("En proceso",F3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H38">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Bajo">
+      <formula>NOT(ISERROR(SEARCH("Bajo",H3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Medio">
+      <formula>NOT(ISERROR(SEARCH("Medio",H3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Alto">
+      <formula>NOT(ISERROR(SEARCH("Alto",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Plan de pruebas v1.0.4
</commit_message>
<xml_diff>
--- a/Plan de pruebas/Plan de pruebas - The internet.xlsx
+++ b/Plan de pruebas/Plan de pruebas - The internet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Titulo del caso de prueba</t>
   </si>
@@ -454,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -494,9 +494,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -523,21 +520,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -548,14 +531,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -563,13 +539,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -888,7 +857,7 @@
   <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +887,7 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -938,13 +907,13 @@
       <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -961,13 +930,13 @@
       <c r="E4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -984,13 +953,13 @@
       <c r="E5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1007,13 +976,13 @@
       <c r="E6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1030,13 +999,13 @@
       <c r="E7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1053,13 +1022,13 @@
       <c r="E8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1076,11 +1045,11 @@
       <c r="E9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="18" t="s">
+      <c r="G9" s="13"/>
+      <c r="H9" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1097,11 +1066,11 @@
       <c r="E10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="18" t="s">
+      <c r="G10" s="13"/>
+      <c r="H10" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1118,11 +1087,13 @@
       <c r="E11" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="18" t="s">
+      <c r="F11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1131,267 +1102,267 @@
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="16"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="16"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="16"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="16"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="16"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="16"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="16"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="16"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="16"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="16"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="16"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="16"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="16"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="16"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="15"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="16"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="16"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
       <c r="D28" s="11"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="16"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="16"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="16"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="11"/>
       <c r="E31" s="12"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="16"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
       <c r="D32" s="11"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="16"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="9"/>
       <c r="C33" s="10"/>
       <c r="D33" s="11"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="16"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="15"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="16"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="15"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="16"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="15"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="12"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="16"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="15"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
       <c r="C37" s="10"/>
       <c r="D37" s="11"/>
       <c r="E37" s="12"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="16"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="15"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
       <c r="C38" s="10"/>
       <c r="D38" s="11"/>
       <c r="E38" s="12"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="16"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F38">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Exitosa">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Exitosa">
       <formula>NOT(ISERROR(SEARCH("Exitosa",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Fallida">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Fallida">
       <formula>NOT(ISERROR(SEARCH("Fallida",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Exitosa con observaciones">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Exitosa con observaciones">
       <formula>NOT(ISERROR(SEARCH("Exitosa con observaciones",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="En proceso">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="En proceso">
       <formula>NOT(ISERROR(SEARCH("En proceso",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H38">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Bajo">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Bajo">
       <formula>NOT(ISERROR(SEARCH("Bajo",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Medio">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medio">
       <formula>NOT(ISERROR(SEARCH("Medio",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Alto">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Alto">
       <formula>NOT(ISERROR(SEARCH("Alto",H3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Plan de pruebas v1.0.5
</commit_message>
<xml_diff>
--- a/Plan de pruebas/Plan de pruebas - The internet.xlsx
+++ b/Plan de pruebas/Plan de pruebas - The internet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\portafolio\Pruebas-Selenium-java\Plan de pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seba\Desktop\portafolio\Pruebas-Selenium-java\Plan de pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5A239A-24A0-4EA1-BF95-618C7CB503B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4575"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de pruebas" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>Titulo del caso de prueba</t>
   </si>
@@ -92,9 +93,6 @@
     <t xml:space="preserve">Todas las imágenes de la pagina cargan correctamente  </t>
   </si>
   <si>
-    <t>Fallida</t>
-  </si>
-  <si>
     <t>CP-001 A/B Testing</t>
   </si>
   <si>
@@ -137,9 +135,6 @@
   </si>
   <si>
     <t>CP-006</t>
-  </si>
-  <si>
-    <t>Issues: 2 de las imágenes no cargan correctamente</t>
   </si>
   <si>
     <t>CP-007 Drag and drop</t>
@@ -210,12 +205,39 @@
   <si>
     <t>Medio</t>
   </si>
+  <si>
+    <t>PAU-01</t>
+  </si>
+  <si>
+    <t>PAU-03</t>
+  </si>
+  <si>
+    <t>PAU-02</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>PAU-04</t>
+  </si>
+  <si>
+    <t>PAU-05</t>
+  </si>
+  <si>
+    <t>PAU-06</t>
+  </si>
+  <si>
+    <t>Fallido</t>
+  </si>
+  <si>
+    <t>Issue: PAU-07 "Error - Imágenes no cargan correctamente"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +274,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -273,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -340,19 +368,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -450,11 +465,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -462,65 +576,109 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -531,6 +689,48 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -538,6 +738,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
@@ -545,28 +773,42 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -853,11 +1095,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,8 +1112,8 @@
     <col min="7" max="7" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -890,13 +1132,16 @@
       <c r="G2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
@@ -907,19 +1152,22 @@
       <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>9</v>
+      <c r="F3" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="101.25" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>11</v>
@@ -930,19 +1178,22 @@
       <c r="E4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>9</v>
+      <c r="F4" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="H4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>14</v>
@@ -953,22 +1204,25 @@
       <c r="E5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>9</v>
+      <c r="F5" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="H5" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>18</v>
@@ -976,394 +1230,434 @@
       <c r="E6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>19</v>
+      <c r="F6" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="67.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="67.5" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H7" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="E8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>9</v>
+        <v>31</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="H8" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="191.25" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="E9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="F9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="2:9" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="2:9" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="C11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="E11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="17" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="19"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="21"/>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="19"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="21"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="19"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="21"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="19"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="21"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="19"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="21"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="19"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="21"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="19"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="21"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
-      <c r="F19" s="19"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="21"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="19"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="21"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="19"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="21"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="19"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="21"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="19"/>
+      <c r="F23" s="17"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="21"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="19"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="21"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="19"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="21"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="19"/>
+      <c r="F26" s="17"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="21"/>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
-      <c r="F27" s="19"/>
+      <c r="F27" s="17"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="21"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
       <c r="D28" s="11"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="19"/>
+      <c r="F28" s="17"/>
       <c r="G28" s="13"/>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="21"/>
+      <c r="I28" s="15"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
-      <c r="F29" s="19"/>
+      <c r="F29" s="17"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="21"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
-      <c r="F30" s="19"/>
+      <c r="F30" s="17"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="21"/>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="11"/>
       <c r="E31" s="12"/>
-      <c r="F31" s="19"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="13"/>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="21"/>
+      <c r="I31" s="15"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="9"/>
       <c r="C32" s="10"/>
       <c r="D32" s="11"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="19"/>
+      <c r="F32" s="17"/>
       <c r="G32" s="13"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="21"/>
+      <c r="I32" s="15"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="9"/>
       <c r="C33" s="10"/>
       <c r="D33" s="11"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="19"/>
+      <c r="F33" s="17"/>
       <c r="G33" s="13"/>
-      <c r="H33" s="15"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="21"/>
+      <c r="I33" s="15"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
-      <c r="F34" s="19"/>
+      <c r="F34" s="17"/>
       <c r="G34" s="13"/>
-      <c r="H34" s="15"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="21"/>
+      <c r="I34" s="15"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
-      <c r="F35" s="19"/>
+      <c r="F35" s="17"/>
       <c r="G35" s="13"/>
-      <c r="H35" s="15"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="21"/>
+      <c r="I35" s="15"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="12"/>
-      <c r="F36" s="19"/>
+      <c r="F36" s="17"/>
       <c r="G36" s="13"/>
-      <c r="H36" s="15"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="21"/>
+      <c r="I36" s="15"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
       <c r="C37" s="10"/>
       <c r="D37" s="11"/>
       <c r="E37" s="12"/>
-      <c r="F37" s="19"/>
+      <c r="F37" s="17"/>
       <c r="G37" s="13"/>
-      <c r="H37" s="15"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="15"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="15"/>
+    </row>
+    <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="23"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="F3:F38">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Exitosa">
-      <formula>NOT(ISERROR(SEARCH("Exitosa",F3)))</formula>
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="En proceso">
+      <formula>NOT(ISERROR(SEARCH("En proceso",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Fallida">
-      <formula>NOT(ISERROR(SEARCH("Fallida",F3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Exitosa con observaciones">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Exitosa con observaciones">
       <formula>NOT(ISERROR(SEARCH("Exitosa con observaciones",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="En proceso">
-      <formula>NOT(ISERROR(SEARCH("En proceso",F3)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Fallido">
+      <formula>NOT(ISERROR(SEARCH("Fallido",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Finalizado">
+      <formula>NOT(ISERROR(SEARCH("Finalizado",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H38">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Bajo">
-      <formula>NOT(ISERROR(SEARCH("Bajo",H3)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Alto">
+      <formula>NOT(ISERROR(SEARCH("Alto",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medio">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Medio">
       <formula>NOT(ISERROR(SEARCH("Medio",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Alto">
-      <formula>NOT(ISERROR(SEARCH("Alto",H3)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Bajo">
+      <formula>NOT(ISERROR(SEARCH("Bajo",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Plan de pruebas v.1.0.6
</commit_message>
<xml_diff>
--- a/Plan de pruebas/Plan de pruebas - The internet.xlsx
+++ b/Plan de pruebas/Plan de pruebas - The internet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seba\Desktop\portafolio\Pruebas-Selenium-java\Plan de pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seba\Desktop\portafolio\Pruebas-Selenium-java\Pruebas-Selenium-java\Plan de pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5A239A-24A0-4EA1-BF95-618C7CB503B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D71BFF-C0FF-44FB-AC52-E07E30FE5714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de pruebas" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Titulo del caso de prueba</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Estado</t>
-  </si>
-  <si>
-    <t>Exitosa</t>
   </si>
   <si>
     <t>No se presento ningun issue relacionado a la prueba</t>
@@ -231,6 +228,15 @@
   </si>
   <si>
     <t>Issue: PAU-07 "Error - Imágenes no cargan correctamente"</t>
+  </si>
+  <si>
+    <t>PAU-08</t>
+  </si>
+  <si>
+    <t>PAU-09</t>
+  </si>
+  <si>
+    <t>PAU-10</t>
   </si>
 </sst>
 </file>
@@ -664,105 +670,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -1098,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,15 +1041,15 @@
         <v>4</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
@@ -1153,215 +1061,221 @@
         <v>7</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="101.25" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>16</v>
-      </c>
       <c r="F5" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>57</v>
-      </c>
       <c r="H6" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="67.5" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="E8" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="191.25" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>35</v>
-      </c>
       <c r="F9" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="15"/>
+        <v>47</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>40</v>
-      </c>
       <c r="F10" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="15"/>
+        <v>45</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="2:9" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="F11" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="15"/>
+      <c r="I11" s="15" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
@@ -1636,27 +1550,27 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="F3:F38">
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="En proceso">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="En proceso">
       <formula>NOT(ISERROR(SEARCH("En proceso",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Exitosa con observaciones">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Exitosa con observaciones">
       <formula>NOT(ISERROR(SEARCH("Exitosa con observaciones",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Fallido">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Fallido">
       <formula>NOT(ISERROR(SEARCH("Fallido",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Finalizado">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Finalizado">
       <formula>NOT(ISERROR(SEARCH("Finalizado",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H38">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Alto">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Alto">
       <formula>NOT(ISERROR(SEARCH("Alto",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Medio">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medio">
       <formula>NOT(ISERROR(SEARCH("Medio",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Bajo">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Bajo">
       <formula>NOT(ISERROR(SEARCH("Bajo",H3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>